<commit_message>
Getting MK2 to work with large data set
</commit_message>
<xml_diff>
--- a/TestNotizen.xlsx
+++ b/TestNotizen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunipaderbornde-my.sharepoint.com/personal/sussekl_mail_uni-paderborn_de/Documents/07_SoSe 23/Bachelorarbeit/k2extensions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{BA651EA6-4B92-4EF9-A585-7BBC2EBCB814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59692C49-1F99-462B-BD9C-4B6A992F09CE}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{BA651EA6-4B92-4EF9-A585-7BBC2EBCB814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B48C1F-30E6-47D9-8C35-2E09F63DB868}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65D19FD2-8C61-4E2D-AC31-3E263B82C6CC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>&lt;https://sws.geonames.org/3020251/&gt;</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>&lt;https://www.geonames.org&gt;</t>
+  </si>
+  <si>
+    <t>1100110010001100110010000110110011001001001100000000000000000000</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -217,6 +220,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -535,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D17712-AE7E-44C9-AEDA-4850F27F717D}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,15 +777,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>